<commit_message>
Week_08 project initial commit
</commit_message>
<xml_diff>
--- a/Challenge_AProjectAWeek_Git.xlsx
+++ b/Challenge_AProjectAWeek_Git.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Challenge_AprojectAweek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Challenge_AProjectAWeek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A77A0A5-32A5-4E1A-8BDE-AA49B5008A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B39B486-F3CE-4683-8565-5B3116F50367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -235,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -256,9 +256,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -636,71 +633,71 @@
       <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="8"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>44768</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>0.91666666666666663</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <f t="shared" ref="E4:E12" si="0">D4-C4</f>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <f>SUM(E4:E10)</f>
         <v>0.84374999999999978</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16">
         <v>44769</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <v>0.4375</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>0.52083333333333337</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="18">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21" t="s">
+      <c r="F5" s="19"/>
+      <c r="G5" s="20" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -708,139 +705,139 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17">
+      <c r="A6" s="15"/>
+      <c r="B6" s="16">
         <v>44769</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <v>0.97916666666666663</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="18">
         <f t="shared" si="0"/>
         <v>0.14583333333333326</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20" t="s">
+      <c r="F6" s="19"/>
+      <c r="G6" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16">
         <v>44770</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="17">
         <v>0.5</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="18">
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16">
         <v>44770</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <v>0.85416666666666663</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="18">
         <f t="shared" si="0"/>
         <v>0.14583333333333326</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16">
         <v>44771</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="17">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <v>6.25E-2</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="18">
         <f t="shared" si="0"/>
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23">
+      <c r="A10" s="21"/>
+      <c r="B10" s="22">
         <v>44771</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="23">
         <v>0.6875</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="23">
         <v>0.85416666666666663</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="24">
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="A11" s="9">
         <v>2</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <v>44776</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <v>0.91666666666666663</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="12">
         <f t="shared" si="0"/>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <f>SUM(E11:E16)</f>
         <v>0.74999999999999967</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16">
         <v>44777</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="17">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="17">
         <v>0.8125</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="18">
         <f t="shared" si="0"/>
         <v>0.22916666666666663</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21" t="s">
+      <c r="F12" s="19"/>
+      <c r="G12" s="20" t="s">
         <v>9</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -848,103 +845,103 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17">
+      <c r="A13" s="15"/>
+      <c r="B13" s="16">
         <v>44777</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="17">
         <v>0.89583333333333337</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="17">
         <v>0.97916666666666663</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="18">
         <f t="shared" ref="E13" si="1">D13-C13</f>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20" t="s">
+      <c r="F13" s="19"/>
+      <c r="G13" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="17">
+      <c r="A14" s="15"/>
+      <c r="B14" s="16">
         <v>44778</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="17">
         <v>0.5625</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="17">
         <v>0.72916666666666663</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="18">
         <f t="shared" ref="E14" si="2">D14-C14</f>
         <v>0.16666666666666663</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20" t="s">
+      <c r="F14" s="19"/>
+      <c r="G14" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16">
         <v>44778</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="17">
         <v>0.89583333333333337</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="17">
         <v>0.97916666666666663</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="18">
         <f t="shared" ref="E15" si="3">D15-C15</f>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23">
+      <c r="A16" s="21"/>
+      <c r="B16" s="22">
         <v>44780</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="23">
         <v>0.875</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="23">
         <v>0.97916666666666663</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="24">
         <f t="shared" ref="E16" si="4">D16-C16</f>
         <v>0.10416666666666663</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
+      <c r="A17" s="9">
         <v>3</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <v>44781</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="11">
         <v>0.625</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="12">
         <f t="shared" ref="E17" si="5">D17-C17</f>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="13">
         <f>SUM(E17:E25)</f>
         <v>0.91666666666666663</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="14" t="s">
         <v>13</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -952,22 +949,22 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17">
+      <c r="A18" s="15"/>
+      <c r="B18" s="16">
         <v>44781</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="17">
         <v>0.875</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="17">
         <v>0.91666666666666663</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="18">
         <f t="shared" ref="E18:E19" si="6">D18-C18</f>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="F18" s="20"/>
-      <c r="G18" s="21" t="s">
+      <c r="F18" s="19"/>
+      <c r="G18" s="20" t="s">
         <v>12</v>
       </c>
       <c r="H18" s="1" t="s">
@@ -975,175 +972,175 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17">
+      <c r="A19" s="15"/>
+      <c r="B19" s="16">
         <v>44782</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="17">
         <v>0.625</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="18">
         <f t="shared" si="6"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20" t="s">
+      <c r="F19" s="19"/>
+      <c r="G19" s="19" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17">
+      <c r="A20" s="15"/>
+      <c r="B20" s="16">
         <v>44783</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="17">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="17">
         <v>0.83333333333333337</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="18">
         <f t="shared" ref="E20" si="7">D20-C20</f>
         <v>0.16666666666666674</v>
       </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17">
+      <c r="A21" s="15"/>
+      <c r="B21" s="16">
         <v>44783</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="17">
         <v>0.875</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="17">
         <v>0.97916666666666663</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="18">
         <f t="shared" ref="E21" si="8">D21-C21</f>
         <v>0.10416666666666663</v>
       </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17">
+      <c r="A22" s="15"/>
+      <c r="B22" s="16">
         <v>44784</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="17">
         <v>0.39583333333333331</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="17">
         <v>0.52083333333333337</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="18">
         <f t="shared" ref="E22" si="9">D22-C22</f>
         <v>0.12500000000000006</v>
       </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17">
+      <c r="A23" s="15"/>
+      <c r="B23" s="16">
         <v>44784</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="17">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="17">
         <v>0.83333333333333337</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="18">
         <f t="shared" ref="E23" si="10">D23-C23</f>
         <v>0.16666666666666674</v>
       </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="16"/>
-      <c r="B24" s="17">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16">
         <v>44785</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="17">
         <v>0.375</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="17">
         <v>0.45833333333333331</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="18">
         <f t="shared" ref="E24" si="11">D24-C24</f>
         <v>8.3333333333333315E-2</v>
       </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="22"/>
-      <c r="B25" s="23">
+      <c r="A25" s="21"/>
+      <c r="B25" s="22">
         <v>44785</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C25" s="23">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="23">
         <v>0.6875</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="24">
         <f t="shared" ref="E25" si="12">D25-C25</f>
         <v>0.10416666666666663</v>
       </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="10">
+      <c r="A26" s="9">
         <v>4</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B26" s="10">
         <v>44788</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="11">
         <v>0.5625</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="11">
         <v>0.77083333333333337</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="12">
         <f t="shared" ref="E26" si="13">D26-C26</f>
         <v>0.20833333333333337</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="13">
         <f>SUM(E26:E30)</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="16"/>
-      <c r="B27" s="17">
+      <c r="A27" s="15"/>
+      <c r="B27" s="16">
         <v>44789</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="17">
         <v>0.625</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D27" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E27" s="18">
         <f t="shared" ref="E27" si="14">D27-C27</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="21" t="s">
+      <c r="F27" s="19"/>
+      <c r="G27" s="20" t="s">
         <v>18</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -1151,103 +1148,103 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="16"/>
-      <c r="B28" s="17">
+      <c r="A28" s="15"/>
+      <c r="B28" s="16">
         <v>44789</v>
       </c>
-      <c r="C28" s="18">
+      <c r="C28" s="17">
         <v>0.8125</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="17">
         <v>0.89583333333333337</v>
       </c>
-      <c r="E28" s="19">
+      <c r="E28" s="18">
         <f t="shared" ref="E28" si="15">D28-C28</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20" t="s">
+      <c r="F28" s="19"/>
+      <c r="G28" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
-      <c r="B29" s="17">
+      <c r="A29" s="15"/>
+      <c r="B29" s="16">
         <v>44790</v>
       </c>
-      <c r="C29" s="18">
+      <c r="C29" s="17">
         <v>0.625</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E29" s="19">
+      <c r="E29" s="18">
         <f t="shared" ref="E29" si="16">D29-C29</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="22"/>
-      <c r="B30" s="23">
+      <c r="A30" s="21"/>
+      <c r="B30" s="22">
         <v>44792</v>
       </c>
-      <c r="C30" s="24">
+      <c r="C30" s="23">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="23">
         <v>0.54166666666666663</v>
       </c>
-      <c r="E30" s="25">
+      <c r="E30" s="24">
         <f t="shared" ref="E30" si="17">D30-C30</f>
         <v>8.3333333333333315E-2</v>
       </c>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="10">
+      <c r="A31" s="9">
         <v>5</v>
       </c>
-      <c r="B31" s="11">
+      <c r="B31" s="10">
         <v>44795</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="11">
         <v>0.90625</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="11">
         <v>0.94791666666666663</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="12">
         <f t="shared" ref="E31" si="18">D31-C31</f>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="13">
         <f>SUM(E31:E38)</f>
         <v>0.39583333333333326</v>
       </c>
-      <c r="G31" s="15" t="s">
+      <c r="G31" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="16"/>
-      <c r="B32" s="17">
+      <c r="A32" s="15"/>
+      <c r="B32" s="16">
         <v>44796</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C32" s="17">
         <v>0.4375</v>
       </c>
-      <c r="D32" s="18">
+      <c r="D32" s="17">
         <v>0.51041666666666663</v>
       </c>
-      <c r="E32" s="19">
+      <c r="E32" s="18">
         <f t="shared" ref="E32" si="19">D32-C32</f>
         <v>7.291666666666663E-2</v>
       </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="21" t="s">
+      <c r="F32" s="19"/>
+      <c r="G32" s="20" t="s">
         <v>22</v>
       </c>
       <c r="H32" s="1" t="s">
@@ -1255,133 +1252,133 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
-      <c r="B33" s="17">
+      <c r="A33" s="15"/>
+      <c r="B33" s="16">
         <v>44796</v>
       </c>
-      <c r="C33" s="18">
+      <c r="C33" s="17">
         <v>0.5625</v>
       </c>
-      <c r="D33" s="18">
+      <c r="D33" s="17">
         <v>0.625</v>
       </c>
-      <c r="E33" s="19">
+      <c r="E33" s="18">
         <f t="shared" ref="E33" si="20">D33-C33</f>
         <v>6.25E-2</v>
       </c>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
       <c r="H33" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="16"/>
-      <c r="B34" s="17">
+      <c r="A34" s="15"/>
+      <c r="B34" s="16">
         <v>44796</v>
       </c>
-      <c r="C34" s="18">
+      <c r="C34" s="17">
         <v>0.91666666666666663</v>
       </c>
-      <c r="D34" s="18">
+      <c r="D34" s="17">
         <v>0.94791666666666663</v>
       </c>
-      <c r="E34" s="19">
+      <c r="E34" s="18">
         <f t="shared" ref="E34" si="21">D34-C34</f>
         <v>3.125E-2</v>
       </c>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="16"/>
-      <c r="B35" s="17">
+      <c r="A35" s="15"/>
+      <c r="B35" s="16">
         <v>44797</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="17">
         <v>0.57291666666666663</v>
       </c>
-      <c r="D35" s="18">
+      <c r="D35" s="17">
         <v>0.61458333333333337</v>
       </c>
-      <c r="E35" s="19">
+      <c r="E35" s="18">
         <f t="shared" ref="E35" si="22">D35-C35</f>
         <v>4.1666666666666741E-2</v>
       </c>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="16"/>
-      <c r="B36" s="17">
+      <c r="A36" s="15"/>
+      <c r="B36" s="16">
         <v>44799</v>
       </c>
-      <c r="C36" s="18">
+      <c r="C36" s="17">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D36" s="18">
+      <c r="D36" s="17">
         <v>0.64583333333333337</v>
       </c>
-      <c r="E36" s="19">
+      <c r="E36" s="18">
         <f t="shared" ref="E36" si="23">D36-C36</f>
         <v>6.25E-2</v>
       </c>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="16"/>
-      <c r="B37" s="17">
+      <c r="A37" s="15"/>
+      <c r="B37" s="16">
         <v>44800</v>
       </c>
-      <c r="C37" s="18">
+      <c r="C37" s="17">
         <v>0.89583333333333337</v>
       </c>
-      <c r="D37" s="18">
+      <c r="D37" s="17">
         <v>0.97916666666666663</v>
       </c>
-      <c r="E37" s="19">
+      <c r="E37" s="18">
         <f t="shared" ref="E37" si="24">D37-C37</f>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="16"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="16"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="22"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Finished #8 - Model building: Part I
</commit_message>
<xml_diff>
--- a/Challenge_AProjectAWeek_Git.xlsx
+++ b/Challenge_AProjectAWeek_Git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Challenge_AProjectAWeek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B39B486-F3CE-4683-8565-5B3116F50367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0283822B-0338-4F6A-AB9B-2066B0821500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>Week</t>
   </si>
@@ -49,12 +49,6 @@
     <t>Time end</t>
   </si>
   <si>
-    <t>Time diff. Hrs</t>
-  </si>
-  <si>
-    <t>Project time Hrs</t>
-  </si>
-  <si>
     <t>Project name</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
   </si>
   <si>
     <t>Lesson 1 - Linear Regression with Scikit Learn (Machine Learning with Python: Zero to GBMs)</t>
-  </si>
-  <si>
-    <t>(my project)</t>
   </si>
   <si>
     <t>EDA</t>
@@ -117,11 +108,47 @@
   <si>
     <t>https://www.udemy.com/course/data-analysis-real-world-use-cases-hands-on-python/learn/lecture/24785090#overview</t>
   </si>
+  <si>
+    <t>Time Series Analysis in Python: Master Applied Data Analysis</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/time-series-data-analysis-with-python/learn/lecture/25469760#overview</t>
+  </si>
+  <si>
+    <t>7a</t>
+  </si>
+  <si>
+    <t>Intellipaat Capstone Project 1</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>7b</t>
+  </si>
+  <si>
+    <t>Zomato spatial data analysis</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/spatial-data-science-in-python/learn/lecture/23469402#overview</t>
+  </si>
+  <si>
+    <t>Time Series Analysis</t>
+  </si>
+  <si>
+    <t>Project time hh:mm:ss</t>
+  </si>
+  <si>
+    <t>Time diff. hh:mm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -170,7 +197,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -179,15 +206,24 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="hair">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right style="hair">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -195,6 +231,32 @@
     </border>
     <border>
       <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -208,6 +270,17 @@
     </border>
     <border>
       <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -221,10 +294,68 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right style="hair">
         <color auto="1"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -235,7 +366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -258,11 +389,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -273,44 +407,59 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -599,13 +748,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J35" sqref="J35"/>
+      <selection pane="bottomRight" activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,772 +762,1232 @@
     <col min="1" max="1" width="7.33203125" style="5" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
     <col min="3" max="4" width="10.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.21875" style="1" customWidth="1"/>
     <col min="7" max="7" width="36.109375" style="1" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G1" s="4"/>
-      <c r="I1" s="7"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="14">
         <v>1</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="15">
         <v>44768</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="16">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="16">
         <v>0.91666666666666663</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="17">
         <f t="shared" ref="E4:E12" si="0">D4-C4</f>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="18">
         <f>SUM(E4:E10)</f>
         <v>0.84374999999999978</v>
       </c>
-      <c r="G4" s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16">
+      <c r="G4" s="24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="19"/>
+      <c r="B5" s="8">
         <v>44769</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="9">
         <v>0.4375</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="9">
         <v>0.52083333333333337</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="10">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20" t="s">
-        <v>7</v>
+      <c r="F5" s="20"/>
+      <c r="G5" s="25" t="s">
+        <v>5</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="19"/>
+      <c r="B6" s="8">
         <v>44769</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="9">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="9">
         <v>0.97916666666666663</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="10">
         <f t="shared" si="0"/>
         <v>0.14583333333333326</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16">
+      <c r="F6" s="20"/>
+      <c r="G6" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="19"/>
+      <c r="B7" s="8">
         <v>44770</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="9">
         <v>0.5</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="9">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="10">
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16">
+      <c r="F7" s="20"/>
+      <c r="G7" s="26"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="19"/>
+      <c r="B8" s="8">
         <v>44770</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="9">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="9">
         <v>0.85416666666666663</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="10">
         <f t="shared" si="0"/>
         <v>0.14583333333333326</v>
       </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16">
+      <c r="F8" s="20"/>
+      <c r="G8" s="26"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="19"/>
+      <c r="B9" s="8">
         <v>44771</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="9">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="9">
         <v>6.25E-2</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="10">
         <f t="shared" si="0"/>
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F9" s="20"/>
+      <c r="G9" s="26"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="21"/>
-      <c r="B10" s="22">
+      <c r="B10" s="11">
         <v>44771</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="12">
         <v>0.6875</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="12">
         <v>0.85416666666666663</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="13">
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
+      <c r="F10" s="22"/>
+      <c r="G10" s="27"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
         <v>2</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="15">
         <v>44776</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="16">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="16">
         <v>0.91666666666666663</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="17">
         <f t="shared" si="0"/>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="18">
         <f>SUM(E11:E16)</f>
         <v>0.74999999999999967</v>
       </c>
-      <c r="G11" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16">
+      <c r="G11" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
+      <c r="B12" s="8">
         <v>44777</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="9">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="9">
         <v>0.8125</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="10">
         <f t="shared" si="0"/>
         <v>0.22916666666666663</v>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="20" t="s">
-        <v>9</v>
+      <c r="F12" s="20"/>
+      <c r="G12" s="25" t="s">
+        <v>7</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
+      <c r="B13" s="8">
         <v>44777</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="9">
         <v>0.89583333333333337</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="9">
         <v>0.97916666666666663</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="10">
         <f t="shared" ref="E13" si="1">D13-C13</f>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16">
+      <c r="F13" s="20"/>
+      <c r="G13" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
+      <c r="B14" s="8">
         <v>44778</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="9">
         <v>0.5625</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="9">
         <v>0.72916666666666663</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="10">
         <f t="shared" ref="E14" si="2">D14-C14</f>
         <v>0.16666666666666663</v>
       </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16">
+      <c r="F14" s="20"/>
+      <c r="G14" s="26"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="19"/>
+      <c r="B15" s="8">
         <v>44778</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="9">
         <v>0.89583333333333337</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="9">
         <v>0.97916666666666663</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="10">
         <f t="shared" ref="E15" si="3">D15-C15</f>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F15" s="20"/>
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="21"/>
-      <c r="B16" s="22">
+      <c r="B16" s="11">
         <v>44780</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="12">
         <v>0.875</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="12">
         <v>0.97916666666666663</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="13">
         <f t="shared" ref="E16" si="4">D16-C16</f>
         <v>0.10416666666666663</v>
       </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
+      <c r="A17" s="14">
         <v>3</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="15">
         <v>44781</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="16">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="16">
         <v>0.625</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="17">
         <f t="shared" ref="E17" si="5">D17-C17</f>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="18">
         <f>SUM(E17:E25)</f>
         <v>0.91666666666666663</v>
       </c>
-      <c r="G17" s="14" t="s">
-        <v>13</v>
+      <c r="G17" s="24" t="s">
+        <v>11</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16">
+      <c r="A18" s="19"/>
+      <c r="B18" s="8">
         <v>44781</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="9">
         <v>0.875</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="9">
         <v>0.91666666666666663</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="10">
         <f t="shared" ref="E18:E19" si="6">D18-C18</f>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="20" t="s">
-        <v>12</v>
+      <c r="F18" s="20"/>
+      <c r="G18" s="25" t="s">
+        <v>10</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16">
+      <c r="A19" s="19"/>
+      <c r="B19" s="8">
         <v>44782</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="9">
         <v>0.625</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="9">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="10">
         <f t="shared" si="6"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19" t="s">
-        <v>16</v>
+      <c r="F19" s="20"/>
+      <c r="G19" s="26" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16">
+      <c r="A20" s="19"/>
+      <c r="B20" s="8">
         <v>44783</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="9">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="9">
         <v>0.83333333333333337</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="10">
         <f t="shared" ref="E20" si="7">D20-C20</f>
         <v>0.16666666666666674</v>
       </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16">
+      <c r="A21" s="19"/>
+      <c r="B21" s="8">
         <v>44783</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="9">
         <v>0.875</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="9">
         <v>0.97916666666666663</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="10">
         <f t="shared" ref="E21" si="8">D21-C21</f>
         <v>0.10416666666666663</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16">
+      <c r="A22" s="19"/>
+      <c r="B22" s="8">
         <v>44784</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="9">
         <v>0.39583333333333331</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="9">
         <v>0.52083333333333337</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="10">
         <f t="shared" ref="E22" si="9">D22-C22</f>
         <v>0.12500000000000006</v>
       </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="26"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16">
+      <c r="A23" s="19"/>
+      <c r="B23" s="8">
         <v>44784</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="9">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="9">
         <v>0.83333333333333337</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="10">
         <f t="shared" ref="E23" si="10">D23-C23</f>
         <v>0.16666666666666674</v>
       </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="26"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
-      <c r="B24" s="16">
+      <c r="A24" s="19"/>
+      <c r="B24" s="8">
         <v>44785</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="9">
         <v>0.375</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="9">
         <v>0.45833333333333331</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="10">
         <f t="shared" ref="E24" si="11">D24-C24</f>
         <v>8.3333333333333315E-2</v>
       </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="21"/>
-      <c r="B25" s="22">
+      <c r="B25" s="11">
         <v>44785</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C25" s="12">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="12">
         <v>0.6875</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E25" s="13">
         <f t="shared" ref="E25" si="12">D25-C25</f>
         <v>0.10416666666666663</v>
       </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="27"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="9">
+      <c r="A26" s="14">
         <v>4</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="15">
         <v>44788</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="16">
         <v>0.5625</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="16">
         <v>0.77083333333333337</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="17">
         <f t="shared" ref="E26" si="13">D26-C26</f>
         <v>0.20833333333333337</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="18">
         <f>SUM(E26:E30)</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="G26" s="14" t="s">
-        <v>19</v>
+      <c r="G26" s="24" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
-      <c r="B27" s="16">
+      <c r="A27" s="19"/>
+      <c r="B27" s="8">
         <v>44789</v>
       </c>
-      <c r="C27" s="17">
+      <c r="C27" s="9">
         <v>0.625</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="9">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E27" s="10">
         <f t="shared" ref="E27" si="14">D27-C27</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="20" t="s">
-        <v>18</v>
+      <c r="F27" s="20"/>
+      <c r="G27" s="25" t="s">
+        <v>15</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16">
+      <c r="A28" s="19"/>
+      <c r="B28" s="8">
         <v>44789</v>
       </c>
-      <c r="C28" s="17">
+      <c r="C28" s="9">
         <v>0.8125</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="9">
         <v>0.89583333333333337</v>
       </c>
-      <c r="E28" s="18">
+      <c r="E28" s="10">
         <f t="shared" ref="E28" si="15">D28-C28</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19" t="s">
-        <v>15</v>
+      <c r="F28" s="20"/>
+      <c r="G28" s="26" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="15"/>
-      <c r="B29" s="16">
+      <c r="A29" s="19"/>
+      <c r="B29" s="8">
         <v>44790</v>
       </c>
-      <c r="C29" s="17">
+      <c r="C29" s="9">
         <v>0.625</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="9">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E29" s="18">
+      <c r="E29" s="10">
         <f t="shared" ref="E29" si="16">D29-C29</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="26"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="21"/>
-      <c r="B30" s="22">
+      <c r="B30" s="11">
         <v>44792</v>
       </c>
-      <c r="C30" s="23">
+      <c r="C30" s="12">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D30" s="23">
+      <c r="D30" s="12">
         <v>0.54166666666666663</v>
       </c>
-      <c r="E30" s="24">
+      <c r="E30" s="13">
         <f t="shared" ref="E30" si="17">D30-C30</f>
         <v>8.3333333333333315E-2</v>
       </c>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="27"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="9">
+      <c r="A31" s="14">
         <v>5</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="15">
         <v>44795</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="16">
         <v>0.90625</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="16">
         <v>0.94791666666666663</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="17">
         <f t="shared" ref="E31" si="18">D31-C31</f>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="F31" s="13">
-        <f>SUM(E31:E38)</f>
-        <v>0.39583333333333326</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>21</v>
+      <c r="F31" s="18">
+        <f>SUM(E31:E40)</f>
+        <v>0.62499999999999989</v>
+      </c>
+      <c r="G31" s="24" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
-      <c r="B32" s="16">
+      <c r="A32" s="19"/>
+      <c r="B32" s="8">
         <v>44796</v>
       </c>
-      <c r="C32" s="17">
+      <c r="C32" s="9">
         <v>0.4375</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="9">
         <v>0.51041666666666663</v>
       </c>
-      <c r="E32" s="18">
+      <c r="E32" s="10">
         <f t="shared" ref="E32" si="19">D32-C32</f>
         <v>7.291666666666663E-2</v>
       </c>
-      <c r="F32" s="19"/>
-      <c r="G32" s="20" t="s">
-        <v>22</v>
+      <c r="F32" s="20"/>
+      <c r="G32" s="25" t="s">
+        <v>19</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="15"/>
-      <c r="B33" s="16">
+      <c r="A33" s="19"/>
+      <c r="B33" s="8">
         <v>44796</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C33" s="9">
         <v>0.5625</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="9">
         <v>0.625</v>
       </c>
-      <c r="E33" s="18">
+      <c r="E33" s="10">
         <f t="shared" ref="E33" si="20">D33-C33</f>
         <v>6.25E-2</v>
       </c>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="1" t="s">
-        <v>8</v>
+      <c r="F33" s="20"/>
+      <c r="G33" s="26" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="15"/>
-      <c r="B34" s="16">
+      <c r="A34" s="19"/>
+      <c r="B34" s="8">
         <v>44796</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="9">
         <v>0.91666666666666663</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="9">
         <v>0.94791666666666663</v>
       </c>
-      <c r="E34" s="18">
+      <c r="E34" s="10">
         <f t="shared" ref="E34" si="21">D34-C34</f>
         <v>3.125E-2</v>
       </c>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="26"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16">
+      <c r="A35" s="19"/>
+      <c r="B35" s="8">
         <v>44797</v>
       </c>
-      <c r="C35" s="17">
+      <c r="C35" s="9">
         <v>0.57291666666666663</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="9">
         <v>0.61458333333333337</v>
       </c>
-      <c r="E35" s="18">
+      <c r="E35" s="10">
         <f t="shared" ref="E35" si="22">D35-C35</f>
         <v>4.1666666666666741E-2</v>
       </c>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="26"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="15"/>
-      <c r="B36" s="16">
+      <c r="A36" s="19"/>
+      <c r="B36" s="8">
         <v>44799</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C36" s="9">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="9">
         <v>0.64583333333333337</v>
       </c>
-      <c r="E36" s="18">
+      <c r="E36" s="10">
         <f t="shared" ref="E36" si="23">D36-C36</f>
         <v>6.25E-2</v>
       </c>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="26"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="15"/>
-      <c r="B37" s="16">
+      <c r="A37" s="19"/>
+      <c r="B37" s="8">
         <v>44800</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C37" s="9">
         <v>0.89583333333333337</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="9">
         <v>0.97916666666666663</v>
       </c>
-      <c r="E37" s="18">
-        <f t="shared" ref="E37" si="24">D37-C37</f>
+      <c r="E37" s="10">
+        <f t="shared" ref="E37:E56" si="24">D37-C37</f>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="26"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
+      <c r="A38" s="19"/>
+      <c r="B38" s="8">
+        <v>44812</v>
+      </c>
+      <c r="C38" s="9">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D38" s="9">
+        <v>0.53125</v>
+      </c>
+      <c r="E38" s="10">
+        <f t="shared" si="24"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="F38" s="20"/>
+      <c r="G38" s="26"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="8">
+        <v>44812</v>
+      </c>
+      <c r="C39" s="9">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D39" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="E39" s="10">
+        <f t="shared" si="24"/>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="F39" s="20"/>
+      <c r="G39" s="26"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="11">
+        <v>44812</v>
+      </c>
+      <c r="C40" s="12">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="D40" s="12">
+        <v>0.90625</v>
+      </c>
+      <c r="E40" s="13">
+        <f t="shared" si="24"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F40" s="22"/>
+      <c r="G40" s="27"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="21"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
+      <c r="A41" s="14">
+        <v>6</v>
+      </c>
+      <c r="B41" s="15">
+        <v>44802</v>
+      </c>
+      <c r="C41" s="16">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D41" s="16">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="E41" s="17">
+        <f t="shared" si="24"/>
+        <v>8.3333333333333259E-2</v>
+      </c>
+      <c r="F41" s="18">
+        <f>SUM(E41:E54)</f>
+        <v>1.354166666666667</v>
+      </c>
+      <c r="G41" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="19"/>
+      <c r="B42" s="8">
+        <v>44803</v>
+      </c>
+      <c r="C42" s="9">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D42" s="9">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="E42" s="10">
+        <f t="shared" si="24"/>
+        <v>0.13541666666666669</v>
+      </c>
+      <c r="F42" s="20"/>
+      <c r="G42" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="19"/>
+      <c r="B43" s="8">
+        <v>44803</v>
+      </c>
+      <c r="C43" s="9">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D43" s="9">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="E43" s="10">
+        <f t="shared" si="24"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F43" s="20"/>
+      <c r="G43" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="19"/>
+      <c r="B44" s="8">
+        <v>44803</v>
+      </c>
+      <c r="C44" s="9">
+        <v>0.875</v>
+      </c>
+      <c r="D44" s="9">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="E44" s="10">
+        <f t="shared" si="24"/>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="F44" s="20"/>
+      <c r="G44" s="26"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="19"/>
+      <c r="B45" s="8">
+        <v>44804</v>
+      </c>
+      <c r="C45" s="9">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D45" s="9">
+        <v>0.8125</v>
+      </c>
+      <c r="E45" s="10">
+        <f t="shared" si="24"/>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="F45" s="20"/>
+      <c r="G45" s="26"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="19"/>
+      <c r="B46" s="8">
+        <v>44804</v>
+      </c>
+      <c r="C46" s="9">
+        <v>0.90625</v>
+      </c>
+      <c r="D46" s="9">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="E46" s="10">
+        <f t="shared" si="24"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F46" s="20"/>
+      <c r="G46" s="26"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="19"/>
+      <c r="B47" s="8">
+        <v>44805</v>
+      </c>
+      <c r="C47" s="9">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D47" s="9">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E47" s="10">
+        <f t="shared" si="24"/>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="F47" s="20"/>
+      <c r="G47" s="26"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="19"/>
+      <c r="B48" s="8">
+        <v>44805</v>
+      </c>
+      <c r="C48" s="9">
+        <v>0.625</v>
+      </c>
+      <c r="D48" s="9">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="E48" s="10">
+        <f t="shared" si="24"/>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="F48" s="20"/>
+      <c r="G48" s="26"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="19"/>
+      <c r="B49" s="8">
+        <v>44805</v>
+      </c>
+      <c r="C49" s="9">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="D49" s="9">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="E49" s="10">
+        <f t="shared" si="24"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="F49" s="20"/>
+      <c r="G49" s="26"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="19"/>
+      <c r="B50" s="8">
+        <v>44807</v>
+      </c>
+      <c r="C50" s="9">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D50" s="9">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="E50" s="10">
+        <f t="shared" si="24"/>
+        <v>0.16666666666666674</v>
+      </c>
+      <c r="F50" s="20"/>
+      <c r="G50" s="26"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="19"/>
+      <c r="B51" s="8">
+        <v>44808</v>
+      </c>
+      <c r="C51" s="9">
+        <v>0.71875</v>
+      </c>
+      <c r="D51" s="9">
+        <v>0.78125</v>
+      </c>
+      <c r="E51" s="10">
+        <f t="shared" si="24"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F51" s="20"/>
+      <c r="G51" s="26"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="19"/>
+      <c r="B52" s="8">
+        <v>44808</v>
+      </c>
+      <c r="C52" s="9">
+        <v>0.90625</v>
+      </c>
+      <c r="D52" s="9">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="E52" s="10">
+        <f t="shared" si="24"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F52" s="20"/>
+      <c r="G52" s="26"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="19"/>
+      <c r="B53" s="8">
+        <v>44810</v>
+      </c>
+      <c r="C53" s="9">
+        <v>0.875</v>
+      </c>
+      <c r="D53" s="9">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E53" s="10">
+        <f t="shared" si="24"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F53" s="20"/>
+      <c r="G53" s="26"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="21"/>
+      <c r="B54" s="11">
+        <v>44811</v>
+      </c>
+      <c r="C54" s="12">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D54" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="E54" s="13">
+        <f t="shared" si="24"/>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="F54" s="22"/>
+      <c r="G54" s="27"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" s="15">
+        <v>44809</v>
+      </c>
+      <c r="C55" s="16">
+        <v>0.46875</v>
+      </c>
+      <c r="D55" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="E55" s="17">
+        <f t="shared" si="24"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F55" s="18">
+        <f>SUM(E55:E56)</f>
+        <v>0.10416666666666674</v>
+      </c>
+      <c r="G55" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="19"/>
+      <c r="B56" s="8">
+        <v>44809</v>
+      </c>
+      <c r="C56" s="9">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D56" s="9">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="E56" s="10">
+        <f t="shared" si="24"/>
+        <v>7.2916666666666741E-2</v>
+      </c>
+      <c r="F56" s="20"/>
+      <c r="G56" s="26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="21"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="27"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B58" s="15">
+        <v>44810</v>
+      </c>
+      <c r="C58" s="16">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D58" s="16">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="E58" s="17">
+        <f t="shared" ref="E58:E63" si="25">D58-C58</f>
+        <v>5.2083333333333259E-2</v>
+      </c>
+      <c r="F58" s="18">
+        <f>SUM(E58:E63)</f>
+        <v>0.36458333333333326</v>
+      </c>
+      <c r="G58" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" s="23"/>
+      <c r="B59" s="8">
+        <v>44810</v>
+      </c>
+      <c r="C59" s="9">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D59" s="9">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E59" s="10">
+        <f t="shared" si="25"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="F59" s="20"/>
+      <c r="G59" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="19"/>
+      <c r="B60" s="8">
+        <v>44810</v>
+      </c>
+      <c r="C60" s="9">
+        <v>0.8125</v>
+      </c>
+      <c r="D60" s="9">
+        <v>0.875</v>
+      </c>
+      <c r="E60" s="10">
+        <f t="shared" si="25"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F60" s="20"/>
+      <c r="G60" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="19"/>
+      <c r="B61" s="8">
+        <v>44811</v>
+      </c>
+      <c r="C61" s="9">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D61" s="9">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E61" s="10">
+        <f t="shared" si="25"/>
+        <v>0.10416666666666669</v>
+      </c>
+      <c r="F61" s="20"/>
+      <c r="G61" s="26"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="19"/>
+      <c r="B62" s="8">
+        <v>44811</v>
+      </c>
+      <c r="C62" s="9">
+        <v>0.875</v>
+      </c>
+      <c r="D62" s="9">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E62" s="10">
+        <f t="shared" si="25"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F62" s="20"/>
+      <c r="G62" s="26"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="21"/>
+      <c r="B63" s="11">
+        <v>44812</v>
+      </c>
+      <c r="C63" s="12">
+        <v>0.3125</v>
+      </c>
+      <c r="D63" s="12">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E63" s="13">
+        <f t="shared" si="25"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="F63" s="22"/>
+      <c r="G63" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1387,8 +1996,10 @@
     <hyperlink ref="G18" r:id="rId3" display="https://jovian.ai/learn/machine-learning-with-python-zero-to-gbms/lesson/linear-regression-with-scikit-learn (Machine Learning with Python: Zero to GBMs)" xr:uid="{DCE1A9C6-C4D4-4597-B08A-32A5AF851874}"/>
     <hyperlink ref="G27" r:id="rId4" location="overview" xr:uid="{0FF06D1B-50DB-42AA-83AA-9FCD772C34FE}"/>
     <hyperlink ref="G32" r:id="rId5" location="overview" xr:uid="{D047A7DF-B14B-45E0-8D43-54C4D645BD09}"/>
+    <hyperlink ref="G42" r:id="rId6" location="overview" xr:uid="{36D172E4-3C97-486F-83D0-EF9C4CD80CF1}"/>
+    <hyperlink ref="G59" r:id="rId7" location="overview" xr:uid="{C24B3A1A-29E8-4C97-BA10-2044094FFE3E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Week_8 and Week_9 projects
</commit_message>
<xml_diff>
--- a/Challenge_AProjectAWeek_Git.xlsx
+++ b/Challenge_AProjectAWeek_Git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Challenge_AProjectAWeek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0283822B-0338-4F6A-AB9B-2066B0821500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF552184-3DAE-4517-9E0E-AF6EC6C3991E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>Week</t>
   </si>
@@ -140,6 +140,30 @@
   </si>
   <si>
     <t>Time diff. hh:mm</t>
+  </si>
+  <si>
+    <t>Loan Prediction ML Project</t>
+  </si>
+  <si>
+    <t>Analytics Vidhya</t>
+  </si>
+  <si>
+    <t>ML - Classification</t>
+  </si>
+  <si>
+    <t>https://datahack.analyticsvidhya.com/contest/practice-problem-loan-prediction-iii/#DiscussTab</t>
+  </si>
+  <si>
+    <t>Predict the price of Bitcoin</t>
+  </si>
+  <si>
+    <t>Udemy</t>
+  </si>
+  <si>
+    <t>Time Series</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/time-series-analysis-real-world-use-cases-in-python/learn/lecture/28361560#overview</t>
   </si>
 </sst>
 </file>
@@ -366,7 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -448,9 +472,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -748,13 +769,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C52" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K56" sqref="K56"/>
+      <selection pane="bottomRight" activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,25 +803,25 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="30" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="7"/>
@@ -1814,7 +1835,7 @@
       <c r="G54" s="27"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="28" t="s">
+      <c r="A55" s="14" t="s">
         <v>22</v>
       </c>
       <c r="B55" s="15">
@@ -1881,7 +1902,7 @@
         <v>0.69791666666666663</v>
       </c>
       <c r="E58" s="17">
-        <f t="shared" ref="E58:E63" si="25">D58-C58</f>
+        <f t="shared" ref="E58:E71" si="25">D58-C58</f>
         <v>5.2083333333333259E-2</v>
       </c>
       <c r="F58" s="18">
@@ -1988,6 +2009,434 @@
       </c>
       <c r="F63" s="22"/>
       <c r="G63" s="27"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" s="14">
+        <v>8</v>
+      </c>
+      <c r="B64" s="15">
+        <v>44816</v>
+      </c>
+      <c r="C64" s="16">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D64" s="16">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E64" s="17">
+        <f t="shared" si="25"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F64" s="18">
+        <f>SUM(E64:E76)</f>
+        <v>1.322916666666667</v>
+      </c>
+      <c r="G64" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" s="19"/>
+      <c r="B65" s="8">
+        <v>44816</v>
+      </c>
+      <c r="C65" s="9">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D65" s="9">
+        <v>0.8125</v>
+      </c>
+      <c r="E65" s="10">
+        <f t="shared" si="25"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F65" s="20"/>
+      <c r="G65" s="26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="19"/>
+      <c r="B66" s="8">
+        <v>44817</v>
+      </c>
+      <c r="C66" s="9">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D66" s="9">
+        <v>0.5625</v>
+      </c>
+      <c r="E66" s="10">
+        <f t="shared" si="25"/>
+        <v>0.14583333333333331</v>
+      </c>
+      <c r="F66" s="20"/>
+      <c r="G66" s="26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" s="19"/>
+      <c r="B67" s="8">
+        <v>44818</v>
+      </c>
+      <c r="C67" s="9">
+        <v>0.40625</v>
+      </c>
+      <c r="D67" s="9">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E67" s="10">
+        <f t="shared" si="25"/>
+        <v>0.11458333333333337</v>
+      </c>
+      <c r="F67" s="20"/>
+      <c r="G67" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" s="19"/>
+      <c r="B68" s="8">
+        <v>44818</v>
+      </c>
+      <c r="C68" s="9">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D68" s="9">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E68" s="10">
+        <f t="shared" si="25"/>
+        <v>0.10416666666666674</v>
+      </c>
+      <c r="F68" s="20"/>
+      <c r="G68" s="26"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" s="19"/>
+      <c r="B69" s="8">
+        <v>44819</v>
+      </c>
+      <c r="C69" s="9">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D69" s="9">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E69" s="10">
+        <f t="shared" si="25"/>
+        <v>0.12499999999999994</v>
+      </c>
+      <c r="F69" s="20"/>
+      <c r="G69" s="26"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="19"/>
+      <c r="B70" s="8">
+        <v>44820</v>
+      </c>
+      <c r="C70" s="9">
+        <v>0.4375</v>
+      </c>
+      <c r="D70" s="9">
+        <v>0.53125</v>
+      </c>
+      <c r="E70" s="10">
+        <f t="shared" si="25"/>
+        <v>9.375E-2</v>
+      </c>
+      <c r="F70" s="20"/>
+      <c r="G70" s="26"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="19"/>
+      <c r="B71" s="8">
+        <v>44820</v>
+      </c>
+      <c r="C71" s="9">
+        <v>0.5625</v>
+      </c>
+      <c r="D71" s="9">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="E71" s="10">
+        <f t="shared" si="25"/>
+        <v>0.23958333333333337</v>
+      </c>
+      <c r="F71" s="20"/>
+      <c r="G71" s="26"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" s="19"/>
+      <c r="B72" s="8">
+        <v>44821</v>
+      </c>
+      <c r="C72" s="9">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="D72" s="9">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="E72" s="10">
+        <f>D72-C72</f>
+        <v>0.125</v>
+      </c>
+      <c r="F72" s="20"/>
+      <c r="G72" s="25"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" s="19"/>
+      <c r="B73" s="8">
+        <v>44822</v>
+      </c>
+      <c r="C73" s="9">
+        <v>0.71875</v>
+      </c>
+      <c r="D73" s="9">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="E73" s="10">
+        <f>D73-C73</f>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="F73" s="20"/>
+      <c r="G73" s="26"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" s="19"/>
+      <c r="B74" s="8">
+        <v>44822</v>
+      </c>
+      <c r="C74" s="9">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="D74" s="9">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="E74" s="10">
+        <f>D74-C74</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F74" s="20"/>
+      <c r="G74" s="25"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" s="19"/>
+      <c r="B75" s="8">
+        <v>44825</v>
+      </c>
+      <c r="C75" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="D75" s="9">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="E75" s="10">
+        <f>D75-C75</f>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="F75" s="20"/>
+      <c r="G75" s="26"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" s="19"/>
+      <c r="B76" s="8">
+        <v>44825</v>
+      </c>
+      <c r="C76" s="9">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D76" s="9">
+        <v>0.9375</v>
+      </c>
+      <c r="E76" s="10">
+        <f>D76-C76</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F76" s="20"/>
+      <c r="G76" s="26"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" s="14">
+        <v>9</v>
+      </c>
+      <c r="B77" s="15">
+        <v>44823</v>
+      </c>
+      <c r="C77" s="16">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D77" s="16">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E77" s="17">
+        <f t="shared" ref="E77:E85" si="26">D77-C77</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F77" s="18">
+        <f>SUM(E77:E85)</f>
+        <v>0.5625</v>
+      </c>
+      <c r="G77" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78" s="19"/>
+      <c r="B78" s="8">
+        <v>44823</v>
+      </c>
+      <c r="C78" s="9">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D78" s="9">
+        <v>0.65625</v>
+      </c>
+      <c r="E78" s="10">
+        <f t="shared" si="26"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F78" s="20"/>
+      <c r="G78" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79" s="19"/>
+      <c r="B79" s="8">
+        <v>44823</v>
+      </c>
+      <c r="C79" s="9">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D79" s="9">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E79" s="10">
+        <f t="shared" si="26"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="F79" s="20"/>
+      <c r="G79" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80" s="19"/>
+      <c r="B80" s="8">
+        <v>44823</v>
+      </c>
+      <c r="C80" s="9">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D80" s="9">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="E80" s="10">
+        <f t="shared" si="26"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F80" s="20"/>
+      <c r="G80" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" s="19"/>
+      <c r="B81" s="8">
+        <v>44824</v>
+      </c>
+      <c r="C81" s="9">
+        <v>0.65625</v>
+      </c>
+      <c r="D81" s="9">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="E81" s="10">
+        <f t="shared" si="26"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F81" s="20"/>
+      <c r="G81" s="26"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" s="19"/>
+      <c r="B82" s="8">
+        <v>44825</v>
+      </c>
+      <c r="C82" s="9">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D82" s="9">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E82" s="10">
+        <f t="shared" si="26"/>
+        <v>5.2083333333333315E-2</v>
+      </c>
+      <c r="F82" s="20"/>
+      <c r="G82" s="26"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83" s="19"/>
+      <c r="B83" s="8">
+        <v>44825</v>
+      </c>
+      <c r="C83" s="9">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D83" s="9">
+        <v>0.65625</v>
+      </c>
+      <c r="E83" s="10">
+        <f t="shared" si="26"/>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="F83" s="20"/>
+      <c r="G83" s="26"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" s="19"/>
+      <c r="B84" s="8">
+        <v>44826</v>
+      </c>
+      <c r="C84" s="9">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D84" s="9">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E84" s="10">
+        <f t="shared" si="26"/>
+        <v>0.11458333333333331</v>
+      </c>
+      <c r="F84" s="20"/>
+      <c r="G84" s="26"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" s="21"/>
+      <c r="B85" s="11">
+        <v>44826</v>
+      </c>
+      <c r="C85" s="12">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D85" s="12">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E85" s="13">
+        <f t="shared" si="26"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F85" s="22"/>
+      <c r="G85" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1998,8 +2447,10 @@
     <hyperlink ref="G32" r:id="rId5" location="overview" xr:uid="{D047A7DF-B14B-45E0-8D43-54C4D645BD09}"/>
     <hyperlink ref="G42" r:id="rId6" location="overview" xr:uid="{36D172E4-3C97-486F-83D0-EF9C4CD80CF1}"/>
     <hyperlink ref="G59" r:id="rId7" location="overview" xr:uid="{C24B3A1A-29E8-4C97-BA10-2044094FFE3E}"/>
+    <hyperlink ref="G67" r:id="rId8" location="DiscussTab" xr:uid="{F6CC8730-F915-4260-9C5D-A3C08078E37C}"/>
+    <hyperlink ref="G80" r:id="rId9" location="overview" xr:uid="{F02C4AAD-D900-402D-ABA1-D1F64F18FA8B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Week_11 project initial commit
</commit_message>
<xml_diff>
--- a/Challenge_AProjectAWeek_Git.xlsx
+++ b/Challenge_AProjectAWeek_Git.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Challenge_AProjectAWeek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF552184-3DAE-4517-9E0E-AF6EC6C3991E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BD4D3C-AE4F-4A7D-8B2D-25726FD0CBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>Week</t>
   </si>
@@ -52,24 +52,15 @@
     <t>Project name</t>
   </si>
   <si>
-    <t>https://www.kaggle.com/datasets/sobhanmoosavi/us-accidents?select=US_Accidents_Dec21_updated.csv</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>https://www.ucsusa.org/resources/satellite-database#.VF_jIlPF8Wg</t>
-  </si>
-  <si>
     <t>UCS Satellite Database EDA</t>
   </si>
   <si>
     <t>US Accidents EDA</t>
   </si>
   <si>
-    <t>https://jovian.ai/learn/machine-learning-with-python-zero-to-gbms/lesson/linear-regression-with-scikit-learn (https://jovian.ai/learn/machine-learning-with-python-zero-to-gbms)</t>
-  </si>
-  <si>
     <t>Lesson 1 - Linear Regression with Scikit Learn (Machine Learning with Python: Zero to GBMs)</t>
   </si>
   <si>
@@ -80,9 +71,6 @@
   </si>
   <si>
     <t>This is my challenge to complete one project (or some work) a week.</t>
-  </si>
-  <si>
-    <t>https://www.udemy.com/course/data-analysis-real-world-use-cases-hands-on-python/learn/lecture/24786280#overview</t>
   </si>
   <si>
     <t>Finance DA - Bank Loan</t>
@@ -106,15 +94,9 @@
     <t>Amazon customer data analysis</t>
   </si>
   <si>
-    <t>https://www.udemy.com/course/data-analysis-real-world-use-cases-hands-on-python/learn/lecture/24785090#overview</t>
-  </si>
-  <si>
     <t>Time Series Analysis in Python: Master Applied Data Analysis</t>
   </si>
   <si>
-    <t>https://www.udemy.com/course/time-series-data-analysis-with-python/learn/lecture/25469760#overview</t>
-  </si>
-  <si>
     <t>7a</t>
   </si>
   <si>
@@ -130,9 +112,6 @@
     <t>Zomato spatial data analysis</t>
   </si>
   <si>
-    <t>https://www.udemy.com/course/spatial-data-science-in-python/learn/lecture/23469402#overview</t>
-  </si>
-  <si>
     <t>Time Series Analysis</t>
   </si>
   <si>
@@ -145,25 +124,19 @@
     <t>Loan Prediction ML Project</t>
   </si>
   <si>
-    <t>Analytics Vidhya</t>
-  </si>
-  <si>
     <t>ML - Classification</t>
   </si>
   <si>
-    <t>https://datahack.analyticsvidhya.com/contest/practice-problem-loan-prediction-iii/#DiscussTab</t>
-  </si>
-  <si>
     <t>Predict the price of Bitcoin</t>
   </si>
   <si>
-    <t>Udemy</t>
-  </si>
-  <si>
     <t>Time Series</t>
   </si>
   <si>
-    <t>https://www.udemy.com/course/time-series-analysis-real-world-use-cases-in-python/learn/lecture/28361560#overview</t>
+    <t>Global Warming Analysis</t>
+  </si>
+  <si>
+    <t>Geospatial Data Analysis</t>
   </si>
 </sst>
 </file>
@@ -390,7 +363,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -480,6 +453,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -769,13 +751,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C70" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K85" sqref="K85"/>
+      <selection pane="bottomRight" activeCell="J94" sqref="J94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,14 +773,14 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H2" s="7"/>
     </row>
@@ -816,10 +798,10 @@
         <v>3</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G3" s="30" t="s">
         <v>4</v>
@@ -848,7 +830,7 @@
         <v>0.84374999999999978</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -867,11 +849,11 @@
         <v>8.333333333333337E-2</v>
       </c>
       <c r="F5" s="20"/>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -890,9 +872,7 @@
         <v>0.14583333333333326</v>
       </c>
       <c r="F6" s="20"/>
-      <c r="G6" s="26" t="s">
-        <v>12</v>
-      </c>
+      <c r="G6" s="26"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="19"/>
@@ -988,7 +968,7 @@
         <v>0.74999999999999967</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1007,11 +987,11 @@
         <v>0.22916666666666663</v>
       </c>
       <c r="F12" s="20"/>
-      <c r="G12" s="25" t="s">
-        <v>7</v>
+      <c r="G12" s="26" t="s">
+        <v>9</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1030,9 +1010,7 @@
         <v>8.3333333333333259E-2</v>
       </c>
       <c r="F13" s="20"/>
-      <c r="G13" s="26" t="s">
-        <v>12</v>
-      </c>
+      <c r="G13" s="26"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="19"/>
@@ -1110,10 +1088,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1132,11 +1110,11 @@
         <v>4.166666666666663E-2</v>
       </c>
       <c r="F18" s="20"/>
-      <c r="G18" s="25" t="s">
+      <c r="G18" s="26" t="s">
         <v>10</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1155,9 +1133,7 @@
         <v>8.333333333333337E-2</v>
       </c>
       <c r="F19" s="20"/>
-      <c r="G19" s="26" t="s">
-        <v>13</v>
-      </c>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
@@ -1289,7 +1265,7 @@
         <v>0.54166666666666674</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1308,11 +1284,11 @@
         <v>8.333333333333337E-2</v>
       </c>
       <c r="F27" s="20"/>
-      <c r="G27" s="25" t="s">
-        <v>15</v>
+      <c r="G27" s="26" t="s">
+        <v>9</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -1331,9 +1307,7 @@
         <v>8.333333333333337E-2</v>
       </c>
       <c r="F28" s="20"/>
-      <c r="G28" s="26" t="s">
-        <v>12</v>
-      </c>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
@@ -1393,7 +1367,7 @@
         <v>0.62499999999999989</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -1412,11 +1386,11 @@
         <v>7.291666666666663E-2</v>
       </c>
       <c r="F32" s="20"/>
-      <c r="G32" s="25" t="s">
-        <v>19</v>
+      <c r="G32" s="26" t="s">
+        <v>9</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -1435,9 +1409,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="F33" s="20"/>
-      <c r="G33" s="26" t="s">
-        <v>12</v>
-      </c>
+      <c r="G33" s="26"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="19"/>
@@ -1587,10 +1559,10 @@
         <v>1.354166666666667</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -1609,11 +1581,11 @@
         <v>0.13541666666666669</v>
       </c>
       <c r="F42" s="20"/>
-      <c r="G42" s="25" t="s">
+      <c r="G42" s="26" t="s">
         <v>21</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -1632,9 +1604,7 @@
         <v>3.125E-2</v>
       </c>
       <c r="F43" s="20"/>
-      <c r="G43" s="26" t="s">
-        <v>28</v>
-      </c>
+      <c r="G43" s="26"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="19"/>
@@ -1836,7 +1806,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B55" s="15">
         <v>44809</v>
@@ -1856,7 +1826,7 @@
         <v>0.10416666666666674</v>
       </c>
       <c r="G55" s="24" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -1876,7 +1846,7 @@
       </c>
       <c r="F56" s="20"/>
       <c r="G56" s="26" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
@@ -1890,7 +1860,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B58" s="15">
         <v>44810</v>
@@ -1910,7 +1880,7 @@
         <v>0.36458333333333326</v>
       </c>
       <c r="G58" s="24" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
@@ -1929,11 +1899,11 @@
         <v>2.0833333333333259E-2</v>
       </c>
       <c r="F59" s="20"/>
-      <c r="G59" s="25" t="s">
-        <v>27</v>
+      <c r="G59" s="26" t="s">
+        <v>9</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
@@ -1952,9 +1922,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="F60" s="20"/>
-      <c r="G60" s="26" t="s">
-        <v>12</v>
-      </c>
+      <c r="G60" s="26"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="19"/>
@@ -2032,7 +2000,7 @@
         <v>1.322916666666667</v>
       </c>
       <c r="G64" s="24" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
@@ -2052,7 +2020,7 @@
       </c>
       <c r="F65" s="20"/>
       <c r="G65" s="26" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
@@ -2071,9 +2039,7 @@
         <v>0.14583333333333331</v>
       </c>
       <c r="F66" s="20"/>
-      <c r="G66" s="26" t="s">
-        <v>33</v>
-      </c>
+      <c r="G66" s="25"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="19"/>
@@ -2091,11 +2057,9 @@
         <v>0.11458333333333337</v>
       </c>
       <c r="F67" s="20"/>
-      <c r="G67" s="25" t="s">
-        <v>34</v>
-      </c>
+      <c r="G67" s="25"/>
       <c r="H67" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
@@ -2274,7 +2238,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="E77" s="17">
-        <f t="shared" ref="E77:E85" si="26">D77-C77</f>
+        <f t="shared" ref="E77:E91" si="26">D77-C77</f>
         <v>6.25E-2</v>
       </c>
       <c r="F77" s="18">
@@ -2282,7 +2246,7 @@
         <v>0.5625</v>
       </c>
       <c r="G77" s="24" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
@@ -2302,7 +2266,7 @@
       </c>
       <c r="F78" s="20"/>
       <c r="G78" s="26" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
@@ -2321,9 +2285,7 @@
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="F79" s="20"/>
-      <c r="G79" s="26" t="s">
-        <v>37</v>
-      </c>
+      <c r="G79" s="25"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="19"/>
@@ -2341,14 +2303,12 @@
         <v>3.125E-2</v>
       </c>
       <c r="F80" s="20"/>
-      <c r="G80" s="25" t="s">
-        <v>38</v>
-      </c>
+      <c r="G80" s="25"/>
       <c r="H80" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="19"/>
       <c r="B81" s="8">
         <v>44824</v>
@@ -2366,7 +2326,7 @@
       <c r="F81" s="20"/>
       <c r="G81" s="26"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="19"/>
       <c r="B82" s="8">
         <v>44825</v>
@@ -2384,7 +2344,7 @@
       <c r="F82" s="20"/>
       <c r="G82" s="26"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="19"/>
       <c r="B83" s="8">
         <v>44825</v>
@@ -2402,7 +2362,7 @@
       <c r="F83" s="20"/>
       <c r="G83" s="26"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="19"/>
       <c r="B84" s="8">
         <v>44826</v>
@@ -2420,7 +2380,7 @@
       <c r="F84" s="20"/>
       <c r="G84" s="26"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="21"/>
       <c r="B85" s="11">
         <v>44826</v>
@@ -2437,20 +2397,156 @@
       </c>
       <c r="F85" s="22"/>
       <c r="G85" s="27"/>
+      <c r="H85" s="31"/>
+      <c r="I85" s="31"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" s="14">
+        <v>10</v>
+      </c>
+      <c r="B86" s="15">
+        <v>44830</v>
+      </c>
+      <c r="C86" s="16">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D86" s="16">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E86" s="17">
+        <f t="shared" si="26"/>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="F86" s="18">
+        <f>SUM(E86:E91)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G86" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="H86" s="32"/>
+      <c r="I86" s="31"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="19"/>
+      <c r="B87" s="8">
+        <v>44830</v>
+      </c>
+      <c r="C87" s="9">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D87" s="9">
+        <v>0.78125</v>
+      </c>
+      <c r="E87" s="10">
+        <f t="shared" si="26"/>
+        <v>0.19791666666666663</v>
+      </c>
+      <c r="F87" s="20"/>
+      <c r="G87" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="H87" s="33"/>
+      <c r="I87" s="31"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="19"/>
+      <c r="B88" s="8">
+        <v>44831</v>
+      </c>
+      <c r="C88" s="9">
+        <v>0.875</v>
+      </c>
+      <c r="D88" s="9">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E88" s="10">
+        <f t="shared" si="26"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F88" s="20"/>
+      <c r="G88" s="26"/>
+      <c r="H88" s="32"/>
+      <c r="I88" s="31"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" s="19"/>
+      <c r="B89" s="8">
+        <v>44832</v>
+      </c>
+      <c r="C89" s="9">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D89" s="9">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E89" s="10">
+        <f t="shared" si="26"/>
+        <v>0.125</v>
+      </c>
+      <c r="F89" s="20"/>
+      <c r="G89" s="26"/>
+      <c r="H89" s="32"/>
+      <c r="I89" s="31"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="19"/>
+      <c r="B90" s="8">
+        <v>44833</v>
+      </c>
+      <c r="C90" s="9">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="D90" s="9">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E90" s="10">
+        <f t="shared" si="26"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F90" s="20"/>
+      <c r="G90" s="25"/>
+      <c r="H90" s="32"/>
+      <c r="I90" s="31"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" s="21"/>
+      <c r="B91" s="11">
+        <v>44834</v>
+      </c>
+      <c r="C91" s="12">
+        <v>0.6875</v>
+      </c>
+      <c r="D91" s="12">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E91" s="13">
+        <f t="shared" si="26"/>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="F91" s="22"/>
+      <c r="G91" s="27"/>
+      <c r="H91" s="32"/>
+      <c r="I91" s="31"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H92" s="31"/>
+      <c r="I92" s="31"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H93" s="31"/>
+      <c r="I93" s="31"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" xr:uid="{E2A090CE-8C3B-42FE-B6C0-9C715F6F2F36}"/>
-    <hyperlink ref="G12" r:id="rId2" location=".VF_jIlPF8Wg" xr:uid="{EF74C5CF-9C4A-4A8E-8178-E3E6F68F9F4C}"/>
-    <hyperlink ref="G18" r:id="rId3" display="https://jovian.ai/learn/machine-learning-with-python-zero-to-gbms/lesson/linear-regression-with-scikit-learn (Machine Learning with Python: Zero to GBMs)" xr:uid="{DCE1A9C6-C4D4-4597-B08A-32A5AF851874}"/>
-    <hyperlink ref="G27" r:id="rId4" location="overview" xr:uid="{0FF06D1B-50DB-42AA-83AA-9FCD772C34FE}"/>
-    <hyperlink ref="G32" r:id="rId5" location="overview" xr:uid="{D047A7DF-B14B-45E0-8D43-54C4D645BD09}"/>
-    <hyperlink ref="G42" r:id="rId6" location="overview" xr:uid="{36D172E4-3C97-486F-83D0-EF9C4CD80CF1}"/>
-    <hyperlink ref="G59" r:id="rId7" location="overview" xr:uid="{C24B3A1A-29E8-4C97-BA10-2044094FFE3E}"/>
-    <hyperlink ref="G67" r:id="rId8" location="DiscussTab" xr:uid="{F6CC8730-F915-4260-9C5D-A3C08078E37C}"/>
-    <hyperlink ref="G80" r:id="rId9" location="overview" xr:uid="{F02C4AAD-D900-402D-ABA1-D1F64F18FA8B}"/>
+    <hyperlink ref="G12" r:id="rId1" location=".VF_jIlPF8Wg" display="https://www.ucsusa.org/resources/satellite-database#.VF_jIlPF8Wg" xr:uid="{EF74C5CF-9C4A-4A8E-8178-E3E6F68F9F4C}"/>
+    <hyperlink ref="G18" r:id="rId2" display="https://jovian.ai/learn/machine-learning-with-python-zero-to-gbms/lesson/linear-regression-with-scikit-learn (Machine Learning with Python: Zero to GBMs)" xr:uid="{DCE1A9C6-C4D4-4597-B08A-32A5AF851874}"/>
+    <hyperlink ref="G27" r:id="rId3" location="overview" display="https://www.udemy.com/course/data-analysis-real-world-use-cases-hands-on-python/learn/lecture/24786280#overview" xr:uid="{0FF06D1B-50DB-42AA-83AA-9FCD772C34FE}"/>
+    <hyperlink ref="G32" r:id="rId4" location="overview" display="https://www.udemy.com/course/data-analysis-real-world-use-cases-hands-on-python/learn/lecture/24785090#overview" xr:uid="{D047A7DF-B14B-45E0-8D43-54C4D645BD09}"/>
+    <hyperlink ref="G42" r:id="rId5" location="overview" display="https://www.udemy.com/course/time-series-data-analysis-with-python/learn/lecture/25469760#overview" xr:uid="{36D172E4-3C97-486F-83D0-EF9C4CD80CF1}"/>
+    <hyperlink ref="G59" r:id="rId6" location="overview" display="https://www.udemy.com/course/spatial-data-science-in-python/learn/lecture/23469402#overview" xr:uid="{C24B3A1A-29E8-4C97-BA10-2044094FFE3E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Week_12 project initial commit
</commit_message>
<xml_diff>
--- a/Challenge_AProjectAWeek_Git.xlsx
+++ b/Challenge_AProjectAWeek_Git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Challenge_AProjectAWeek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BD4D3C-AE4F-4A7D-8B2D-25726FD0CBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B73BA0C-818D-4900-8809-252D2A1706AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>Week</t>
   </si>
@@ -137,6 +137,10 @@
   </si>
   <si>
     <t>Geospatial Data Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Time Series Analysis Real world use-cases in python</t>
   </si>
 </sst>
 </file>
@@ -194,7 +198,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -358,12 +362,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -455,14 +499,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -751,13 +807,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I93"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C76" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J94" sqref="J94"/>
+      <selection pane="bottomRight" activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2238,7 +2294,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="E77" s="17">
-        <f t="shared" ref="E77:E91" si="26">D77-C77</f>
+        <f t="shared" ref="E77:E101" si="26">D77-C77</f>
         <v>6.25E-2</v>
       </c>
       <c r="F77" s="18">
@@ -2308,7 +2364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="19"/>
       <c r="B81" s="8">
         <v>44824</v>
@@ -2326,7 +2382,7 @@
       <c r="F81" s="20"/>
       <c r="G81" s="26"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="19"/>
       <c r="B82" s="8">
         <v>44825</v>
@@ -2344,7 +2400,7 @@
       <c r="F82" s="20"/>
       <c r="G82" s="26"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="19"/>
       <c r="B83" s="8">
         <v>44825</v>
@@ -2362,7 +2418,7 @@
       <c r="F83" s="20"/>
       <c r="G83" s="26"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="19"/>
       <c r="B84" s="8">
         <v>44826</v>
@@ -2380,7 +2436,7 @@
       <c r="F84" s="20"/>
       <c r="G84" s="26"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="21"/>
       <c r="B85" s="11">
         <v>44826</v>
@@ -2397,10 +2453,8 @@
       </c>
       <c r="F85" s="22"/>
       <c r="G85" s="27"/>
-      <c r="H85" s="31"/>
-      <c r="I85" s="31"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="14">
         <v>10</v>
       </c>
@@ -2424,10 +2478,9 @@
       <c r="G86" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="H86" s="32"/>
-      <c r="I86" s="31"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H86" s="5"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="19"/>
       <c r="B87" s="8">
         <v>44830</v>
@@ -2446,10 +2499,9 @@
       <c r="G87" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H87" s="33"/>
-      <c r="I87" s="31"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H87" s="31"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="19"/>
       <c r="B88" s="8">
         <v>44831</v>
@@ -2466,10 +2518,9 @@
       </c>
       <c r="F88" s="20"/>
       <c r="G88" s="26"/>
-      <c r="H88" s="32"/>
-      <c r="I88" s="31"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H88" s="5"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="19"/>
       <c r="B89" s="8">
         <v>44832</v>
@@ -2486,10 +2537,9 @@
       </c>
       <c r="F89" s="20"/>
       <c r="G89" s="26"/>
-      <c r="H89" s="32"/>
-      <c r="I89" s="31"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H89" s="5"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="19"/>
       <c r="B90" s="8">
         <v>44833</v>
@@ -2506,10 +2556,9 @@
       </c>
       <c r="F90" s="20"/>
       <c r="G90" s="25"/>
-      <c r="H90" s="32"/>
-      <c r="I90" s="31"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H90" s="5"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="21"/>
       <c r="B91" s="11">
         <v>44834</v>
@@ -2525,17 +2574,247 @@
         <v>0.14583333333333337</v>
       </c>
       <c r="F91" s="22"/>
-      <c r="G91" s="27"/>
-      <c r="H91" s="32"/>
-      <c r="I91" s="31"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H92" s="31"/>
-      <c r="I92" s="31"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H93" s="31"/>
-      <c r="I93" s="31"/>
+      <c r="G91" s="33"/>
+      <c r="H91" s="35"/>
+      <c r="I91" s="36"/>
+      <c r="J91" s="36"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92" s="14">
+        <v>11</v>
+      </c>
+      <c r="B92" s="15">
+        <v>44837</v>
+      </c>
+      <c r="C92" s="16">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D92" s="16">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E92" s="17">
+        <f t="shared" si="26"/>
+        <v>6.2500000000000056E-2</v>
+      </c>
+      <c r="F92" s="18">
+        <f>SUM(E92:E101)</f>
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="G92" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="H92" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="I92" s="36"/>
+      <c r="J92" s="36"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" s="19"/>
+      <c r="B93" s="8">
+        <v>44837</v>
+      </c>
+      <c r="C93" s="9">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D93" s="9">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E93" s="10">
+        <f t="shared" si="26"/>
+        <v>8.3333333333333259E-2</v>
+      </c>
+      <c r="F93" s="32"/>
+      <c r="G93" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="H93" s="35"/>
+      <c r="I93" s="36"/>
+      <c r="J93" s="36"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94" s="19"/>
+      <c r="B94" s="8">
+        <v>44839</v>
+      </c>
+      <c r="C94" s="9">
+        <v>0.90625</v>
+      </c>
+      <c r="D94" s="9">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="E94" s="10">
+        <f t="shared" si="26"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F94" s="32"/>
+      <c r="G94" s="32"/>
+      <c r="H94" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="I94" s="36"/>
+      <c r="J94" s="36"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95" s="19"/>
+      <c r="B95" s="8">
+        <v>44840</v>
+      </c>
+      <c r="C95" s="9">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D95" s="9">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E95" s="10">
+        <f t="shared" si="26"/>
+        <v>8.3333333333333259E-2</v>
+      </c>
+      <c r="F95" s="32"/>
+      <c r="G95" s="32"/>
+      <c r="H95" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="I95" s="36"/>
+      <c r="J95" s="36"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A96" s="19"/>
+      <c r="B96" s="8">
+        <v>44840</v>
+      </c>
+      <c r="C96" s="9">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D96" s="9">
+        <v>0.71875</v>
+      </c>
+      <c r="E96" s="10">
+        <f t="shared" si="26"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F96" s="32"/>
+      <c r="G96" s="32"/>
+      <c r="H96" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="I96" s="36"/>
+      <c r="J96" s="36"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A97" s="19"/>
+      <c r="B97" s="8">
+        <v>44841</v>
+      </c>
+      <c r="C97" s="9">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D97" s="9">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E97" s="10">
+        <f t="shared" si="26"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="F97" s="32"/>
+      <c r="G97" s="32"/>
+      <c r="H97" s="35"/>
+      <c r="I97" s="36"/>
+      <c r="J97" s="36"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A98" s="19"/>
+      <c r="B98" s="8">
+        <v>44841</v>
+      </c>
+      <c r="C98" s="9">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D98" s="9">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="E98" s="10">
+        <f t="shared" si="26"/>
+        <v>0.22916666666666674</v>
+      </c>
+      <c r="F98" s="32"/>
+      <c r="G98" s="32"/>
+      <c r="H98" s="35"/>
+      <c r="I98" s="36"/>
+      <c r="J98" s="36"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A99" s="19"/>
+      <c r="B99" s="8">
+        <v>44841</v>
+      </c>
+      <c r="C99" s="9">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="D99" s="9">
+        <v>0.9375</v>
+      </c>
+      <c r="E99" s="10">
+        <f t="shared" si="26"/>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="F99" s="32"/>
+      <c r="G99" s="32"/>
+      <c r="H99" s="35"/>
+      <c r="I99" s="36"/>
+      <c r="J99" s="36"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A100" s="19"/>
+      <c r="B100" s="8">
+        <v>44842</v>
+      </c>
+      <c r="C100" s="9">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D100" s="9">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E100" s="10">
+        <f t="shared" si="26"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F100" s="32"/>
+      <c r="G100" s="32"/>
+      <c r="H100" s="35"/>
+      <c r="I100" s="36"/>
+      <c r="J100" s="36"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A101" s="21"/>
+      <c r="B101" s="11">
+        <v>44843</v>
+      </c>
+      <c r="C101" s="12">
+        <v>0.71875</v>
+      </c>
+      <c r="D101" s="12">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="E101" s="13">
+        <f t="shared" si="26"/>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="F101" s="33"/>
+      <c r="G101" s="33"/>
+      <c r="H101" s="35"/>
+      <c r="I101" s="36"/>
+      <c r="J101" s="36"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H102" s="37"/>
+      <c r="I102" s="36"/>
+      <c r="J102" s="36"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H103" s="37"/>
+      <c r="I103" s="36"/>
+      <c r="J103" s="36"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Week_13 project initial commit
</commit_message>
<xml_diff>
--- a/Challenge_AProjectAWeek_Git.xlsx
+++ b/Challenge_AProjectAWeek_Git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Challenge_AProjectAWeek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B73BA0C-818D-4900-8809-252D2A1706AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3F05C7-6B2F-46ED-9271-B7B1EB48047F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Week</t>
   </si>
@@ -139,8 +139,10 @@
     <t>Geospatial Data Analysis</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Time Series Analysis Real world use-cases in python</t>
+    <t>Uber New York Data Analysis</t>
+  </si>
+  <si>
+    <t>Predict Number of Births of Babies on a Given Day</t>
   </si>
 </sst>
 </file>
@@ -198,7 +200,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -388,17 +390,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -508,16 +499,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -807,13 +798,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J103"/>
+  <dimension ref="A1:H109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F93" sqref="F93"/>
+      <selection pane="bottomRight" activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2294,7 +2285,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="E77" s="17">
-        <f t="shared" ref="E77:E101" si="26">D77-C77</f>
+        <f t="shared" ref="E77:E109" si="26">D77-C77</f>
         <v>6.25E-2</v>
       </c>
       <c r="F77" s="18">
@@ -2364,7 +2355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="19"/>
       <c r="B81" s="8">
         <v>44824</v>
@@ -2382,7 +2373,7 @@
       <c r="F81" s="20"/>
       <c r="G81" s="26"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="19"/>
       <c r="B82" s="8">
         <v>44825</v>
@@ -2400,7 +2391,7 @@
       <c r="F82" s="20"/>
       <c r="G82" s="26"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="19"/>
       <c r="B83" s="8">
         <v>44825</v>
@@ -2418,7 +2409,7 @@
       <c r="F83" s="20"/>
       <c r="G83" s="26"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="19"/>
       <c r="B84" s="8">
         <v>44826</v>
@@ -2436,7 +2427,7 @@
       <c r="F84" s="20"/>
       <c r="G84" s="26"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="21"/>
       <c r="B85" s="11">
         <v>44826</v>
@@ -2454,7 +2445,7 @@
       <c r="F85" s="22"/>
       <c r="G85" s="27"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="14">
         <v>10</v>
       </c>
@@ -2480,7 +2471,7 @@
       </c>
       <c r="H86" s="5"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="19"/>
       <c r="B87" s="8">
         <v>44830</v>
@@ -2501,7 +2492,7 @@
       </c>
       <c r="H87" s="31"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="19"/>
       <c r="B88" s="8">
         <v>44831</v>
@@ -2520,7 +2511,7 @@
       <c r="G88" s="26"/>
       <c r="H88" s="5"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="19"/>
       <c r="B89" s="8">
         <v>44832</v>
@@ -2539,7 +2530,7 @@
       <c r="G89" s="26"/>
       <c r="H89" s="5"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="19"/>
       <c r="B90" s="8">
         <v>44833</v>
@@ -2558,7 +2549,7 @@
       <c r="G90" s="25"/>
       <c r="H90" s="5"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="21"/>
       <c r="B91" s="11">
         <v>44834</v>
@@ -2575,11 +2566,9 @@
       </c>
       <c r="F91" s="22"/>
       <c r="G91" s="33"/>
-      <c r="H91" s="35"/>
-      <c r="I91" s="36"/>
-      <c r="J91" s="36"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H91" s="34"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="14">
         <v>11</v>
       </c>
@@ -2600,16 +2589,14 @@
         <f>SUM(E92:E101)</f>
         <v>0.77083333333333337</v>
       </c>
-      <c r="G92" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="H92" s="35" t="s">
+      <c r="G92" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="H92" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I92" s="36"/>
-      <c r="J92" s="36"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="19"/>
       <c r="B93" s="8">
         <v>44837</v>
@@ -2628,11 +2615,9 @@
       <c r="G93" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="H93" s="35"/>
-      <c r="I93" s="36"/>
-      <c r="J93" s="36"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H93" s="34"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="19"/>
       <c r="B94" s="8">
         <v>44839</v>
@@ -2649,13 +2634,11 @@
       </c>
       <c r="F94" s="32"/>
       <c r="G94" s="32"/>
-      <c r="H94" s="35" t="s">
+      <c r="H94" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I94" s="36"/>
-      <c r="J94" s="36"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="19"/>
       <c r="B95" s="8">
         <v>44840</v>
@@ -2672,13 +2655,11 @@
       </c>
       <c r="F95" s="32"/>
       <c r="G95" s="32"/>
-      <c r="H95" s="35" t="s">
+      <c r="H95" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I95" s="36"/>
-      <c r="J95" s="36"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="19"/>
       <c r="B96" s="8">
         <v>44840</v>
@@ -2695,13 +2676,11 @@
       </c>
       <c r="F96" s="32"/>
       <c r="G96" s="32"/>
-      <c r="H96" s="35" t="s">
+      <c r="H96" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I96" s="36"/>
-      <c r="J96" s="36"/>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="19"/>
       <c r="B97" s="8">
         <v>44841</v>
@@ -2718,11 +2697,9 @@
       </c>
       <c r="F97" s="32"/>
       <c r="G97" s="32"/>
-      <c r="H97" s="35"/>
-      <c r="I97" s="36"/>
-      <c r="J97" s="36"/>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H97" s="34"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="19"/>
       <c r="B98" s="8">
         <v>44841</v>
@@ -2739,11 +2716,9 @@
       </c>
       <c r="F98" s="32"/>
       <c r="G98" s="32"/>
-      <c r="H98" s="35"/>
-      <c r="I98" s="36"/>
-      <c r="J98" s="36"/>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H98" s="34"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="19"/>
       <c r="B99" s="8">
         <v>44841</v>
@@ -2760,11 +2735,9 @@
       </c>
       <c r="F99" s="32"/>
       <c r="G99" s="32"/>
-      <c r="H99" s="35"/>
-      <c r="I99" s="36"/>
-      <c r="J99" s="36"/>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H99" s="34"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="19"/>
       <c r="B100" s="8">
         <v>44842</v>
@@ -2781,11 +2754,9 @@
       </c>
       <c r="F100" s="32"/>
       <c r="G100" s="32"/>
-      <c r="H100" s="35"/>
-      <c r="I100" s="36"/>
-      <c r="J100" s="36"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H100" s="34"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="21"/>
       <c r="B101" s="11">
         <v>44843</v>
@@ -2802,19 +2773,162 @@
       </c>
       <c r="F101" s="33"/>
       <c r="G101" s="33"/>
-      <c r="H101" s="35"/>
-      <c r="I101" s="36"/>
-      <c r="J101" s="36"/>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H102" s="37"/>
-      <c r="I102" s="36"/>
-      <c r="J102" s="36"/>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H103" s="37"/>
-      <c r="I103" s="36"/>
-      <c r="J103" s="36"/>
+      <c r="H101" s="34"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" s="14">
+        <v>12</v>
+      </c>
+      <c r="B102" s="15">
+        <v>44844</v>
+      </c>
+      <c r="C102" s="16">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D102" s="16">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E102" s="17">
+        <f t="shared" si="26"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F102" s="18">
+        <f>SUM(E102:E109)</f>
+        <v>0.38541666666666663</v>
+      </c>
+      <c r="G102" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="H102" s="35"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A103" s="19"/>
+      <c r="B103" s="8">
+        <v>44844</v>
+      </c>
+      <c r="C103" s="9">
+        <v>0.90625</v>
+      </c>
+      <c r="D103" s="9">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="E103" s="10">
+        <f t="shared" si="26"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F103" s="32"/>
+      <c r="G103" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="H103" s="35"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A104" s="19"/>
+      <c r="B104" s="8">
+        <v>44845</v>
+      </c>
+      <c r="C104" s="9">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D104" s="9">
+        <v>0.9375</v>
+      </c>
+      <c r="E104" s="10">
+        <f t="shared" si="26"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F104" s="32"/>
+      <c r="G104" s="37"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A105" s="19"/>
+      <c r="B105" s="8">
+        <v>44846</v>
+      </c>
+      <c r="C105" s="9">
+        <v>0.875</v>
+      </c>
+      <c r="D105" s="9">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E105" s="10">
+        <f t="shared" si="26"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F105" s="32"/>
+      <c r="G105" s="37"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A106" s="19"/>
+      <c r="B106" s="8">
+        <v>44847</v>
+      </c>
+      <c r="C106" s="9">
+        <v>0.84375</v>
+      </c>
+      <c r="D106" s="9">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E106" s="10">
+        <f t="shared" si="26"/>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="F106" s="32"/>
+      <c r="G106" s="20"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A107" s="19"/>
+      <c r="B107" s="8">
+        <v>44848</v>
+      </c>
+      <c r="C107" s="9">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D107" s="9">
+        <v>0.9375</v>
+      </c>
+      <c r="E107" s="10">
+        <f t="shared" si="26"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F107" s="32"/>
+      <c r="G107" s="20"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A108" s="19"/>
+      <c r="B108" s="8">
+        <v>44849</v>
+      </c>
+      <c r="C108" s="9">
+        <v>0.9375</v>
+      </c>
+      <c r="D108" s="9">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E108" s="10">
+        <f t="shared" si="26"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F108" s="32"/>
+      <c r="G108" s="20"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A109" s="21"/>
+      <c r="B109" s="11">
+        <v>44850</v>
+      </c>
+      <c r="C109" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="D109" s="12">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E109" s="13">
+        <f t="shared" si="26"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F109" s="33"/>
+      <c r="G109" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Week_14 project initial commit
</commit_message>
<xml_diff>
--- a/Challenge_AProjectAWeek_Git.xlsx
+++ b/Challenge_AProjectAWeek_Git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Challenge_AProjectAWeek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3F05C7-6B2F-46ED-9271-B7B1EB48047F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E7B56F-2BF6-46A7-BEB7-A77964C24AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>Week</t>
   </si>
@@ -143,6 +143,15 @@
   </si>
   <si>
     <t>Predict Number of Births of Babies on a Given Day</t>
+  </si>
+  <si>
+    <t>Predict the Prices of Stocks</t>
+  </si>
+  <si>
+    <t>Power BI tutorials</t>
+  </si>
+  <si>
+    <t>-- Enterprise DNA (enterprisedna.co)</t>
   </si>
 </sst>
 </file>
@@ -200,7 +209,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -364,41 +373,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -493,22 +473,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -798,13 +763,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H109"/>
+  <dimension ref="A1:H123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C79" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G92" sqref="G92"/>
+      <selection pane="bottomRight" activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2285,7 +2250,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="E77" s="17">
-        <f t="shared" ref="E77:E109" si="26">D77-C77</f>
+        <f t="shared" ref="E77:E115" si="26">D77-C77</f>
         <v>6.25E-2</v>
       </c>
       <c r="F77" s="18">
@@ -2565,8 +2530,8 @@
         <v>0.14583333333333337</v>
       </c>
       <c r="F91" s="22"/>
-      <c r="G91" s="33"/>
-      <c r="H91" s="34"/>
+      <c r="G91" s="27"/>
+      <c r="H91" s="5"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="14">
@@ -2589,10 +2554,10 @@
         <f>SUM(E92:E101)</f>
         <v>0.77083333333333337</v>
       </c>
-      <c r="G92" s="36" t="s">
+      <c r="G92" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="H92" s="34" t="s">
+      <c r="H92" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2611,11 +2576,11 @@
         <f t="shared" si="26"/>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="F93" s="32"/>
-      <c r="G93" s="32" t="s">
+      <c r="F93" s="20"/>
+      <c r="G93" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="H93" s="34"/>
+      <c r="H93" s="5"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="19"/>
@@ -2632,9 +2597,9 @@
         <f t="shared" si="26"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="F94" s="32"/>
-      <c r="G94" s="32"/>
-      <c r="H94" s="34" t="s">
+      <c r="F94" s="20"/>
+      <c r="G94" s="26"/>
+      <c r="H94" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2653,9 +2618,9 @@
         <f t="shared" si="26"/>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="F95" s="32"/>
-      <c r="G95" s="32"/>
-      <c r="H95" s="34" t="s">
+      <c r="F95" s="20"/>
+      <c r="G95" s="26"/>
+      <c r="H95" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2674,9 +2639,9 @@
         <f t="shared" si="26"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="F96" s="32"/>
-      <c r="G96" s="32"/>
-      <c r="H96" s="34" t="s">
+      <c r="F96" s="20"/>
+      <c r="G96" s="26"/>
+      <c r="H96" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2695,9 +2660,9 @@
         <f t="shared" si="26"/>
         <v>4.1666666666666685E-2</v>
       </c>
-      <c r="F97" s="32"/>
-      <c r="G97" s="32"/>
-      <c r="H97" s="34"/>
+      <c r="F97" s="20"/>
+      <c r="G97" s="26"/>
+      <c r="H97" s="5"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="19"/>
@@ -2714,9 +2679,9 @@
         <f t="shared" si="26"/>
         <v>0.22916666666666674</v>
       </c>
-      <c r="F98" s="32"/>
-      <c r="G98" s="32"/>
-      <c r="H98" s="34"/>
+      <c r="F98" s="20"/>
+      <c r="G98" s="26"/>
+      <c r="H98" s="5"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="19"/>
@@ -2733,9 +2698,9 @@
         <f t="shared" si="26"/>
         <v>5.208333333333337E-2</v>
       </c>
-      <c r="F99" s="32"/>
-      <c r="G99" s="32"/>
-      <c r="H99" s="34"/>
+      <c r="F99" s="20"/>
+      <c r="G99" s="26"/>
+      <c r="H99" s="5"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="19"/>
@@ -2752,9 +2717,9 @@
         <f t="shared" si="26"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="F100" s="32"/>
-      <c r="G100" s="32"/>
-      <c r="H100" s="34"/>
+      <c r="F100" s="20"/>
+      <c r="G100" s="26"/>
+      <c r="H100" s="5"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="21"/>
@@ -2771,9 +2736,9 @@
         <f t="shared" si="26"/>
         <v>5.208333333333337E-2</v>
       </c>
-      <c r="F101" s="33"/>
-      <c r="G101" s="33"/>
-      <c r="H101" s="34"/>
+      <c r="F101" s="22"/>
+      <c r="G101" s="27"/>
+      <c r="H101" s="5"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="14">
@@ -2796,10 +2761,9 @@
         <f>SUM(E102:E109)</f>
         <v>0.38541666666666663</v>
       </c>
-      <c r="G102" s="36" t="s">
+      <c r="G102" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H102" s="35"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="19"/>
@@ -2816,11 +2780,10 @@
         <f t="shared" si="26"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="F103" s="32"/>
+      <c r="F103" s="20"/>
       <c r="G103" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="H103" s="35"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="19"/>
@@ -2837,8 +2800,8 @@
         <f t="shared" si="26"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="F104" s="32"/>
-      <c r="G104" s="37"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="25"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="19"/>
@@ -2855,8 +2818,8 @@
         <f t="shared" si="26"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="F105" s="32"/>
-      <c r="G105" s="37"/>
+      <c r="F105" s="20"/>
+      <c r="G105" s="25"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="19"/>
@@ -2873,8 +2836,8 @@
         <f t="shared" si="26"/>
         <v>5.208333333333337E-2</v>
       </c>
-      <c r="F106" s="32"/>
-      <c r="G106" s="20"/>
+      <c r="F106" s="20"/>
+      <c r="G106" s="26"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="19"/>
@@ -2891,8 +2854,8 @@
         <f t="shared" si="26"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="F107" s="32"/>
-      <c r="G107" s="20"/>
+      <c r="F107" s="20"/>
+      <c r="G107" s="26"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="19"/>
@@ -2909,8 +2872,8 @@
         <f t="shared" si="26"/>
         <v>2.083333333333337E-2</v>
       </c>
-      <c r="F108" s="32"/>
-      <c r="G108" s="20"/>
+      <c r="F108" s="20"/>
+      <c r="G108" s="26"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="21"/>
@@ -2927,8 +2890,214 @@
         <f t="shared" si="26"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="F109" s="33"/>
-      <c r="G109" s="22"/>
+      <c r="F109" s="22"/>
+      <c r="G109" s="27"/>
+      <c r="H109" s="5"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A110" s="14">
+        <v>13</v>
+      </c>
+      <c r="B110" s="15">
+        <v>44851</v>
+      </c>
+      <c r="C110" s="16">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D110" s="16">
+        <v>0.8125</v>
+      </c>
+      <c r="E110" s="17">
+        <f t="shared" si="26"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F110" s="18">
+        <f>SUM(E110:E116)</f>
+        <v>0.27083333333333337</v>
+      </c>
+      <c r="G110" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="H110" s="5"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A111" s="19"/>
+      <c r="B111" s="8">
+        <v>44853</v>
+      </c>
+      <c r="C111" s="9">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D111" s="9">
+        <v>0.875</v>
+      </c>
+      <c r="E111" s="10">
+        <f t="shared" si="26"/>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="F111" s="20"/>
+      <c r="G111" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H111" s="5"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A112" s="19"/>
+      <c r="B112" s="8">
+        <v>44854</v>
+      </c>
+      <c r="C112" s="9">
+        <v>0.78125</v>
+      </c>
+      <c r="D112" s="9">
+        <v>0.84375</v>
+      </c>
+      <c r="E112" s="10">
+        <f t="shared" si="26"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F112" s="20"/>
+      <c r="G112" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A113" s="19"/>
+      <c r="B113" s="8">
+        <v>44856</v>
+      </c>
+      <c r="C113" s="9">
+        <v>0.90625</v>
+      </c>
+      <c r="D113" s="9">
+        <v>0.9375</v>
+      </c>
+      <c r="E113" s="10">
+        <f t="shared" si="26"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F113" s="20"/>
+      <c r="G113" s="25"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A114" s="19"/>
+      <c r="B114" s="8">
+        <v>44857</v>
+      </c>
+      <c r="C114" s="9">
+        <v>0.6875</v>
+      </c>
+      <c r="D114" s="9">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="E114" s="10">
+        <f t="shared" si="26"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F114" s="20"/>
+      <c r="G114" s="25"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A115" s="19"/>
+      <c r="B115" s="8"/>
+      <c r="C115" s="9"/>
+      <c r="D115" s="9"/>
+      <c r="E115" s="10">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="F115" s="20"/>
+      <c r="G115" s="26"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A116" s="21"/>
+      <c r="B116" s="22"/>
+      <c r="C116" s="22"/>
+      <c r="D116" s="22"/>
+      <c r="E116" s="22"/>
+      <c r="F116" s="22"/>
+      <c r="G116" s="27"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A117" s="14">
+        <v>14</v>
+      </c>
+      <c r="B117" s="15">
+        <v>44858</v>
+      </c>
+      <c r="C117" s="16">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D117" s="16">
+        <v>0.9375</v>
+      </c>
+      <c r="E117" s="17">
+        <f t="shared" ref="E117:E123" si="27">D117-C117</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F117" s="18">
+        <f>SUM(E117:E123)</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="G117" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A118" s="19"/>
+      <c r="B118" s="8"/>
+      <c r="C118" s="9"/>
+      <c r="D118" s="9"/>
+      <c r="E118" s="10"/>
+      <c r="F118" s="20"/>
+      <c r="G118" s="32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A119" s="19"/>
+      <c r="B119" s="8"/>
+      <c r="C119" s="9"/>
+      <c r="D119" s="9"/>
+      <c r="E119" s="10"/>
+      <c r="F119" s="20"/>
+      <c r="G119" s="26"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A120" s="19"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="10"/>
+      <c r="F120" s="20"/>
+      <c r="G120" s="25"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A121" s="19"/>
+      <c r="B121" s="8"/>
+      <c r="C121" s="9"/>
+      <c r="D121" s="9"/>
+      <c r="E121" s="10"/>
+      <c r="F121" s="20"/>
+      <c r="G121" s="25"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A122" s="19"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="9"/>
+      <c r="D122" s="9"/>
+      <c r="E122" s="10"/>
+      <c r="F122" s="20"/>
+      <c r="G122" s="26"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A123" s="21"/>
+      <c r="B123" s="22"/>
+      <c r="C123" s="22"/>
+      <c r="D123" s="22"/>
+      <c r="E123" s="22"/>
+      <c r="F123" s="22"/>
+      <c r="G123" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>